<commit_message>
Pardubice - kapacita a denní návštěva, upřesnění
</commit_message>
<xml_diff>
--- a/src/kapacita/navstevnost_existujicich_bazenu.xlsx
+++ b/src/kapacita/navstevnost_existujicich_bazenu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="0" windowWidth="18855" windowHeight="7890"/>
+    <workbookView xWindow="8025" yWindow="0" windowWidth="18855" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Sušice</t>
-  </si>
-  <si>
-    <t>návštěvnost</t>
   </si>
   <si>
     <t>kapacita</t>
@@ -60,12 +57,6 @@
     <t>obyvatel</t>
   </si>
   <si>
-    <t>prům</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
     <t>návštěv za den</t>
   </si>
   <si>
@@ -78,19 +69,46 @@
     <t>denik.cz</t>
   </si>
   <si>
-    <t>pouze bazén 50m. 
-Aktuální vytížení zobrazeno na webu</t>
-  </si>
-  <si>
-    <t>Aquacentrum je komplex 50m bazénu, aquaparku a wellness
-Aktuální vytížení zobrazeno na webu</t>
+    <t>pouze bazén 50m</t>
+  </si>
+  <si>
+    <t>pouze aquapark</t>
+  </si>
+  <si>
+    <t>pouze wellness</t>
+  </si>
+  <si>
+    <t>maps.google.com</t>
+  </si>
+  <si>
+    <t>aktuální počet návštěvníků</t>
+  </si>
+  <si>
+    <t>http://www.aquapce.cz/</t>
+  </si>
+  <si>
+    <t>průměrná</t>
+  </si>
+  <si>
+    <t>max sezóna</t>
+  </si>
+  <si>
+    <t>pouze bazén 50m, nepřesně</t>
+  </si>
+  <si>
+    <t>okamžitá nepřesně. Průměrná vypočtena 
+z roční návštěvy 400 000/365=1095
+Aquacentrum je komplex tří částí:
+- 50m bazén 
+- aquapark
+- wellness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +132,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -129,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -187,6 +213,81 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -194,24 +295,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -221,28 +365,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -639,160 +773,218 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8" customWidth="1"/>
+    <col min="3" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
     <col min="7" max="7" width="40.85546875" customWidth="1"/>
     <col min="8" max="8" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="22"/>
+      <c r="F1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>9</v>
+      <c r="H1" s="23" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:8" s="4" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="4">
         <v>11000</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="4">
         <v>141</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="4">
         <v>420</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="4">
         <v>780</v>
       </c>
-      <c r="F4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>8</v>
+      <c r="F4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="A5" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="18">
         <v>90000</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="11">
         <v>2300</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="1">
         <v>1095</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="17"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="20"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="11">
+        <v>600</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="12">
+        <v>680</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="3">
-        <v>90000</v>
-      </c>
-      <c r="C6" s="3">
-        <v>600</v>
-      </c>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="15" t="s">
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="12">
+        <v>370</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="12">
+        <v>60</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="17"/>
+      <c r="H9" s="15"/>
     </row>
-    <row r="7" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="1"/>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="21"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A5:A10"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="G1:G3"/>
-    <mergeCell ref="D2:E2"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F4" r:id="rId1"/>
     <hyperlink ref="F5" r:id="rId2"/>
     <hyperlink ref="F6" r:id="rId3"/>
+    <hyperlink ref="F7" r:id="rId4"/>
+    <hyperlink ref="F8" r:id="rId5"/>
+    <hyperlink ref="F9" r:id="rId6"/>
+    <hyperlink ref="F10" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Doplněna roční a denní průměrná návštěvnost několika dalších bazénů a vodních center v ČR
</commit_message>
<xml_diff>
--- a/src/kapacita/navstevnost_existujicich_bazenu.xlsx
+++ b/src/kapacita/navstevnost_existujicich_bazenu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="8025" yWindow="0" windowWidth="18855" windowHeight="7890"/>
+    <workbookView xWindow="9630" yWindow="0" windowWidth="18855" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>Sušice</t>
   </si>
@@ -57,9 +57,6 @@
     <t>obyvatel</t>
   </si>
   <si>
-    <t>návštěv za den</t>
-  </si>
-  <si>
     <t>Pardubice</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
   </si>
   <si>
     <t>průměrná</t>
-  </si>
-  <si>
-    <t>max sezóna</t>
   </si>
   <si>
     <t>pouze bazén 50m, nepřesně</t>
@@ -102,6 +96,87 @@
 - 50m bazén 
 - aquapark
 - wellness</t>
+  </si>
+  <si>
+    <t>Praha</t>
+  </si>
+  <si>
+    <t>Bazén Podolí</t>
+  </si>
+  <si>
+    <t>návštěvnost</t>
+  </si>
+  <si>
+    <t>denní</t>
+  </si>
+  <si>
+    <t>roční</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>400 000</t>
+  </si>
+  <si>
+    <t>Aquapalace Čestlice</t>
+  </si>
+  <si>
+    <t>Aquacentrum Pardubice</t>
+  </si>
+  <si>
+    <t>Bazén Slovany</t>
+  </si>
+  <si>
+    <t>Plzeň</t>
+  </si>
+  <si>
+    <t>Bazén Liberec</t>
+  </si>
+  <si>
+    <t>Liberec</t>
+  </si>
+  <si>
+    <t>Bazén Kraví Hora</t>
+  </si>
+  <si>
+    <t>Brno</t>
+  </si>
+  <si>
+    <t>Hradec Králové</t>
+  </si>
+  <si>
+    <t>Uhreské Hradiště</t>
+  </si>
+  <si>
+    <t>Vodní svět</t>
+  </si>
+  <si>
+    <t>Kolín</t>
+  </si>
+  <si>
+    <t>Ostrava</t>
+  </si>
+  <si>
+    <t>Krytý bazén Ostrava Poruba</t>
+  </si>
+  <si>
+    <t>Bazén Uhreské Hradiště</t>
+  </si>
+  <si>
+    <t>Plavecký bazén 50 m</t>
+  </si>
+  <si>
+    <t>průměrná denní výpočtem</t>
+  </si>
+  <si>
+    <t>aquainfo.cz</t>
+  </si>
+  <si>
+    <t>objekt</t>
   </si>
 </sst>
 </file>
@@ -155,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -226,11 +301,26 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -238,30 +328,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -273,7 +339,9 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -281,13 +349,13 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -295,7 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -331,23 +399,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -368,14 +437,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -399,13 +477,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>4229100</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>1352550</xdr:rowOff>
@@ -454,13 +532,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>3933825</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>1066800</xdr:rowOff>
@@ -773,218 +851,496 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A5" sqref="A5:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="10.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="7" max="7" width="40.85546875" customWidth="1"/>
-    <col min="8" max="8" width="67.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+    <col min="9" max="9" width="40.85546875" customWidth="1"/>
+    <col min="10" max="10" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="29"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="27"/>
+      <c r="G2" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="21"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4">
+        <v>11000</v>
+      </c>
+      <c r="D4" s="4">
+        <v>141</v>
+      </c>
+      <c r="E4" s="4">
+        <v>420</v>
+      </c>
+      <c r="F4" s="4">
+        <v>780</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="27" t="s">
+      <c r="C5" s="15">
+        <v>90000</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2300</v>
+      </c>
+      <c r="E5" s="1">
+        <v>1095</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="11">
+        <v>600</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="4">
-        <v>11000</v>
-      </c>
-      <c r="C4" s="4">
-        <v>141</v>
-      </c>
-      <c r="D4" s="4">
-        <v>420</v>
-      </c>
-      <c r="E4" s="4">
-        <v>780</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="18">
-        <v>90000</v>
-      </c>
-      <c r="C5" s="11">
-        <v>2300</v>
-      </c>
-      <c r="D5" s="1">
-        <v>1095</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="8" t="s">
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="12">
+        <v>680</v>
+      </c>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="14"/>
+    </row>
+    <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="30"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="12">
+        <v>370</v>
+      </c>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="14"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="30"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="12">
+        <v>60</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="30"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="11">
-        <v>600</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="12">
-        <v>680</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="15"/>
-    </row>
-    <row r="8" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="12">
-        <v>370</v>
-      </c>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="12">
-        <v>60</v>
-      </c>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="15"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="17"/>
+      <c r="C11" s="9">
+        <v>1280000</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9">
+        <f>ROUNDDOWN(G11/365,-2)</f>
+        <v>2600</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9">
+        <v>960000</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1280000</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9">
+        <f>ROUNDDOWN(G12/365,-2)</f>
+        <v>2200</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9">
+        <v>830000</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="9">
+        <v>170548</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9">
+        <f>ROUNDDOWN(G13/365,-2)</f>
+        <v>1600</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9">
+        <v>600000</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="9">
+        <v>103853</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9">
+        <f>ROUNDDOWN(G14/365,-2)</f>
+        <v>900</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9">
+        <v>355000</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="9">
+        <v>377000</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9">
+        <f>ROUNDDOWN(G15/365,-2)</f>
+        <v>900</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9">
+        <v>350000</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" s="9">
+        <v>92929</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9">
+        <f>ROUNDDOWN(G16/365,-2)</f>
+        <v>900</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9">
+        <v>350000</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="9">
+        <v>25246</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9">
+        <f>ROUNDDOWN(G17/365,-2)</f>
+        <v>900</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9">
+        <v>340000</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="9">
+        <v>31123</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9">
+        <f>ROUNDDOWN(G18/365,-2)</f>
+        <v>700</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9">
+        <v>278000</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="9">
+        <v>291634</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9">
+        <f>ROUNDDOWN(G19/365,-2)</f>
+        <v>700</v>
+      </c>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9">
+        <v>265000</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J19" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="F1:F3"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="H1:H3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="G1:G3"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1"/>
-    <hyperlink ref="F5" r:id="rId2"/>
-    <hyperlink ref="F6" r:id="rId3"/>
-    <hyperlink ref="F7" r:id="rId4"/>
-    <hyperlink ref="F8" r:id="rId5"/>
-    <hyperlink ref="F9" r:id="rId6"/>
-    <hyperlink ref="F10" r:id="rId7"/>
+    <hyperlink ref="H4" r:id="rId1"/>
+    <hyperlink ref="H5" r:id="rId2"/>
+    <hyperlink ref="H6" r:id="rId3"/>
+    <hyperlink ref="H7" r:id="rId4"/>
+    <hyperlink ref="H8" r:id="rId5"/>
+    <hyperlink ref="H9" r:id="rId6"/>
+    <hyperlink ref="H10" r:id="rId7"/>
+    <hyperlink ref="H11" r:id="rId8"/>
+    <hyperlink ref="H12:H19" r:id="rId9" display="aquainfo.cz"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
-  <drawing r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <drawing r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Přidána návštěvnost Bazénu a aquaparku Vyškov
</commit_message>
<xml_diff>
--- a/src/kapacita/navstevnost_existujicich_bazenu.xlsx
+++ b/src/kapacita/navstevnost_existujicich_bazenu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9630" yWindow="0" windowWidth="18855" windowHeight="7890"/>
+    <workbookView xWindow="11235" yWindow="0" windowWidth="18855" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Sušice</t>
   </si>
@@ -177,6 +177,19 @@
   </si>
   <si>
     <t>objekt</t>
+  </si>
+  <si>
+    <t>Vyškov</t>
+  </si>
+  <si>
+    <t>Aquapark Vyškov</t>
+  </si>
+  <si>
+    <t>vyskovsky.denik.cz</t>
+  </si>
+  <si>
+    <t>průměrná denní výpočtem, 
+otevřeno v roce 2001</t>
   </si>
 </sst>
 </file>
@@ -363,7 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -413,13 +426,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -440,20 +465,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -851,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,56 +888,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="27" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="29"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="22" t="s">
+      <c r="F1" s="32"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="26" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="21" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="27"/>
-      <c r="G2" s="28" t="s">
+      <c r="F2" s="31"/>
+      <c r="G2" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="21"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="23"/>
       <c r="E3" s="17" t="s">
         <v>19</v>
       </c>
@@ -927,9 +947,9 @@
       <c r="G3" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
@@ -956,10 +976,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="24" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="15">
@@ -984,8 +1004,8 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="20"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="25"/>
       <c r="C6" s="13"/>
       <c r="D6" s="11">
         <v>600</v>
@@ -1002,8 +1022,8 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="20"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="25"/>
       <c r="C7" s="13"/>
       <c r="D7" s="12">
         <v>680</v>
@@ -1020,8 +1040,8 @@
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="20"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="25"/>
       <c r="C8" s="13"/>
       <c r="D8" s="12">
         <v>370</v>
@@ -1038,8 +1058,8 @@
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="25"/>
       <c r="C9" s="13"/>
       <c r="D9" s="12">
         <v>60</v>
@@ -1056,17 +1076,17 @@
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="25"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="32" t="s">
+      <c r="I10" s="21" t="s">
         <v>17</v>
       </c>
       <c r="J10" s="14"/>
@@ -1083,7 +1103,7 @@
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9">
-        <f>ROUNDDOWN(G11/365,-2)</f>
+        <f t="shared" ref="E11:E20" si="0">ROUNDDOWN(G11/365,-2)</f>
         <v>2600</v>
       </c>
       <c r="F11" s="9"/>
@@ -1110,7 +1130,7 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9">
-        <f>ROUNDDOWN(G12/365,-2)</f>
+        <f t="shared" si="0"/>
         <v>2200</v>
       </c>
       <c r="F12" s="9"/>
@@ -1137,7 +1157,7 @@
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9">
-        <f>ROUNDDOWN(G13/365,-2)</f>
+        <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="F13" s="9"/>
@@ -1164,7 +1184,7 @@
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="9">
-        <f>ROUNDDOWN(G14/365,-2)</f>
+        <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="F14" s="9"/>
@@ -1191,7 +1211,7 @@
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9">
-        <f>ROUNDDOWN(G15/365,-2)</f>
+        <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="F15" s="9"/>
@@ -1218,7 +1238,7 @@
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9">
-        <f>ROUNDDOWN(G16/365,-2)</f>
+        <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="F16" s="9"/>
@@ -1245,7 +1265,7 @@
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9">
-        <f>ROUNDDOWN(G17/365,-2)</f>
+        <f t="shared" si="0"/>
         <v>900</v>
       </c>
       <c r="F17" s="9"/>
@@ -1272,7 +1292,7 @@
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9">
-        <f>ROUNDDOWN(G18/365,-2)</f>
+        <f t="shared" si="0"/>
         <v>700</v>
       </c>
       <c r="F18" s="9"/>
@@ -1299,7 +1319,7 @@
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9">
-        <f>ROUNDDOWN(G19/365,-2)</f>
+        <f t="shared" si="0"/>
         <v>700</v>
       </c>
       <c r="F19" s="9"/>
@@ -1314,19 +1334,46 @@
       </c>
       <c r="J19" s="9"/>
     </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="33">
+        <v>21120</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="33">
+        <f t="shared" si="0"/>
+        <v>600</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="33">
+        <v>240000</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="D2:D3"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1"/>
@@ -1338,9 +1385,10 @@
     <hyperlink ref="H10" r:id="rId7"/>
     <hyperlink ref="H11" r:id="rId8"/>
     <hyperlink ref="H12:H19" r:id="rId9" display="aquainfo.cz"/>
+    <hyperlink ref="H20" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
-  <drawing r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <drawing r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Aktualizovaná návštěvnost Plzeň Slovany podle studie 2009 aktualizovaná verze Němeček https://github.com/janzilka/plavecky-stadion-prostejov/blob/master/src/Plzen-Slovany/2009-studie-aktualizace-nemecek/Baz%C3%A9n%20-%20studie%20-%2004%20-%20hlavn%C3%AD%20probl%C3%A9my.pdf
</commit_message>
<xml_diff>
--- a/src/kapacita/navstevnost_existujicich_bazenu.xlsx
+++ b/src/kapacita/navstevnost_existujicich_bazenu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="0" windowWidth="7650" windowHeight="7890"/>
+    <workbookView xWindow="14370" yWindow="0" windowWidth="7650" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
   <si>
     <t>Sušice</t>
   </si>
@@ -203,6 +203,12 @@
 - 50m bazén 
 - aquapark
 - wellness</t>
+  </si>
+  <si>
+    <t>studie Němeček (2009)</t>
+  </si>
+  <si>
+    <t>průměrná denní výpočtem, důvěryhodnější údaj</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -455,12 +461,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -479,14 +494,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -884,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,7 +912,7 @@
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
-    <col min="9" max="9" width="40.85546875" customWidth="1"/>
+    <col min="9" max="9" width="44.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -907,38 +923,38 @@
       <c r="B1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="30" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="25" t="s">
+      <c r="F1" s="35"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="25" t="s">
+      <c r="J1" s="29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
-      <c r="C2" s="28"/>
+      <c r="C2" s="31"/>
       <c r="D2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="31"/>
+      <c r="F2" s="34"/>
       <c r="G2" s="19" t="s">
         <v>25</v>
       </c>
@@ -949,7 +965,7 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="26"/>
       <c r="B3" s="26"/>
-      <c r="C3" s="29"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="26"/>
       <c r="E3" s="17" t="s">
         <v>19</v>
@@ -989,10 +1005,10 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="27" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="15">
@@ -1017,8 +1033,8 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="13"/>
       <c r="D6" s="11">
         <v>600</v>
@@ -1035,8 +1051,8 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35"/>
-      <c r="B7" s="34"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="13"/>
       <c r="D7" s="12">
         <v>680</v>
@@ -1053,8 +1069,8 @@
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="34"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="13"/>
       <c r="D8" s="12">
         <v>370</v>
@@ -1071,8 +1087,8 @@
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="34"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="13"/>
       <c r="D9" s="12">
         <v>60</v>
@@ -1089,8 +1105,8 @@
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="35"/>
-      <c r="B10" s="34"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="13"/>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -1116,7 +1132,7 @@
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9">
-        <f t="shared" ref="E11:E21" si="0">ROUNDDOWN(G11/365,-2)</f>
+        <f t="shared" ref="E11:E22" si="0">ROUNDDOWN(G11/365,-2)</f>
         <v>2600</v>
       </c>
       <c r="F11" s="9"/>
@@ -1159,22 +1175,22 @@
       <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="27">
         <v>170548</v>
       </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="9">
+      <c r="E13" s="36">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="9">
+      <c r="G13" s="36">
         <v>600000</v>
       </c>
       <c r="H13" s="7" t="s">
@@ -1186,41 +1202,35 @@
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="9">
-        <v>103853</v>
-      </c>
+      <c r="A14" s="37"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="37"/>
       <c r="D14" s="9"/>
       <c r="E14" s="9">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>1200</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="9">
-        <v>355000</v>
+        <v>450000</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="I14" s="9" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C15" s="9">
-        <v>377000</v>
+        <v>103853</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="9">
@@ -1229,7 +1239,7 @@
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="9">
-        <v>350000</v>
+        <v>355000</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>46</v>
@@ -1241,13 +1251,13 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="9">
-        <v>92929</v>
+        <v>377000</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="9">
@@ -1268,13 +1278,13 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="9">
-        <v>25246</v>
+        <v>92929</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="9">
@@ -1283,7 +1293,7 @@
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9">
-        <v>340000</v>
+        <v>350000</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>46</v>
@@ -1295,22 +1305,22 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C18" s="9">
-        <v>31123</v>
+        <v>25246</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9">
-        <v>278000</v>
+        <v>340000</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>46</v>
@@ -1322,13 +1332,13 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="9">
-        <v>291634</v>
+        <v>31123</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9">
@@ -1337,7 +1347,7 @@
       </c>
       <c r="F19" s="9"/>
       <c r="G19" s="9">
-        <v>265000</v>
+        <v>278000</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>46</v>
@@ -1347,75 +1357,105 @@
       </c>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="9">
+        <v>291634</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9">
+        <v>265000</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J20" s="9"/>
+    </row>
+    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B21" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C21" s="22">
         <v>21120</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="22">
+      <c r="D21" s="9"/>
+      <c r="E21" s="22">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="22">
+      <c r="F21" s="9"/>
+      <c r="G21" s="22">
         <v>240000</v>
       </c>
-      <c r="H20" s="23" t="s">
+      <c r="H21" s="23" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="I21" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
+      <c r="J21" s="9"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B22" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C22" s="22">
         <v>43975</v>
       </c>
-      <c r="D21" s="9">
+      <c r="D22" s="9">
         <v>50</v>
       </c>
-      <c r="E21" s="22">
+      <c r="E22" s="22">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="22">
+      <c r="F22" s="9"/>
+      <c r="G22" s="22">
         <v>116000</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H22" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="I22" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J22" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="D2:D3"/>
+  <mergeCells count="14">
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="J1:J3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="D2:D3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1"/>
@@ -1426,12 +1466,13 @@
     <hyperlink ref="H9" r:id="rId6"/>
     <hyperlink ref="H10" r:id="rId7"/>
     <hyperlink ref="H11" r:id="rId8"/>
-    <hyperlink ref="H12:H19" r:id="rId9" display="aquainfo.cz"/>
-    <hyperlink ref="H20" r:id="rId10"/>
-    <hyperlink ref="H21" r:id="rId11"/>
+    <hyperlink ref="H12:H20" r:id="rId9" display="aquainfo.cz"/>
+    <hyperlink ref="H21" r:id="rId10"/>
+    <hyperlink ref="H22" r:id="rId11"/>
+    <hyperlink ref="H14" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
-  <drawing r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dánsko, Kopenhagen - fotografie z realizace Myrtha Pools v ceně 5 mil. EUR (125 mil. Kč) upravena data v dokumentu, který sbírá data o reálné návštěvnosti bazénových center v ČR
</commit_message>
<xml_diff>
--- a/src/kapacita/navstevnost_existujicich_bazenu.xlsx
+++ b/src/kapacita/navstevnost_existujicich_bazenu.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14370" yWindow="0" windowWidth="7650" windowHeight="7890"/>
+    <workbookView xWindow="15900" yWindow="0" windowWidth="7650" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>Sušice</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>poznámka</t>
-  </si>
-  <si>
-    <t>elektronický systém nedovolí vpustit více než maximální počet návštěvníků</t>
   </si>
   <si>
     <t>google "popular times"</t>
@@ -210,12 +207,34 @@
   <si>
     <t>průměrná denní výpočtem, důvěryhodnější údaj</t>
   </si>
+  <si>
+    <t>Bazén Sušice</t>
+  </si>
+  <si>
+    <t>elektronický systém nedovolí vpustit více než maximální počet návštěvníků
+roční návštěva odhad z průměrné denní návštěvy</t>
+  </si>
+  <si>
+    <t>Aquacentrum- bazén 50m</t>
+  </si>
+  <si>
+    <t>Aquacentrum- aquapark</t>
+  </si>
+  <si>
+    <t>Aquacentrum- wellness</t>
+  </si>
+  <si>
+    <t>aktuální data</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="###\ ###\ ##0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +266,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -262,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -390,12 +417,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -404,9 +451,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
@@ -433,9 +477,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,21 +502,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -494,15 +527,43 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -902,14 +963,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="7" width="10.5703125" customWidth="1"/>
     <col min="8" max="8" width="32" customWidth="1"/>
     <col min="9" max="9" width="44.42578125" bestFit="1" customWidth="1"/>
@@ -917,104 +982,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="26" t="s">
+      <c r="A1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="31"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="30"/>
+      <c r="G2" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+    </row>
+    <row r="4" spans="1:10" s="2" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="39">
+        <v>11000</v>
+      </c>
+      <c r="D4" s="3">
+        <v>141</v>
+      </c>
+      <c r="E4" s="3">
+        <v>420</v>
+      </c>
+      <c r="F4" s="3">
+        <v>780</v>
+      </c>
+      <c r="G4" s="14">
+        <f>350*E4</f>
+        <v>147000</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="26"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="26"/>
-    </row>
-    <row r="4" spans="1:10" s="2" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>11000</v>
-      </c>
-      <c r="D4" s="4">
-        <v>141</v>
-      </c>
-      <c r="E4" s="4">
-        <v>420</v>
-      </c>
-      <c r="F4" s="4">
-        <v>780</v>
-      </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="15">
+      <c r="B5" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="43">
         <v>90000</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>2300</v>
       </c>
       <c r="E5" s="1">
@@ -1022,428 +1093,435 @@
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="8"/>
+    </row>
+    <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="37"/>
+      <c r="B6" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="10">
+        <v>600</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="11">
-        <v>600</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="8"/>
+    </row>
+    <row r="7" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="11">
+        <v>680</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="J7" s="13"/>
+    </row>
+    <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37"/>
+      <c r="B8" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="11">
+        <v>370</v>
+      </c>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J8" s="13"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="37"/>
+      <c r="B9" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="44"/>
+      <c r="D9" s="11">
+        <v>60</v>
+      </c>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="13"/>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="37"/>
+      <c r="B10" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="45"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="28"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="12">
-        <v>680</v>
-      </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="14"/>
-    </row>
-    <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="28"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="12">
-        <v>370</v>
-      </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="14"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="12">
-        <v>60</v>
-      </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="14"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="28"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J10" s="14"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="41">
         <v>1280000</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8">
         <f t="shared" ref="E11:E22" si="0">ROUNDDOWN(G11/365,-2)</f>
         <v>2600</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9">
+      <c r="F11" s="8"/>
+      <c r="G11" s="8">
         <v>960000</v>
       </c>
-      <c r="H11" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="9" t="s">
+      <c r="H11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="9"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="9">
-        <v>1280000</v>
-      </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9">
+      <c r="I11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="36"/>
+      <c r="B12" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="42"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8">
         <f t="shared" si="0"/>
         <v>2200</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9">
+      <c r="F12" s="8"/>
+      <c r="G12" s="8">
         <v>830000</v>
       </c>
-      <c r="H12" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="9" t="s">
+      <c r="H12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="I12" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="27">
+      <c r="B13" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="41">
         <v>170548</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="36">
+      <c r="D13" s="8"/>
+      <c r="E13" s="23">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="36">
+      <c r="F13" s="8"/>
+      <c r="G13" s="23">
         <v>600000</v>
       </c>
-      <c r="H13" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="9" t="s">
+      <c r="H13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="9"/>
+      <c r="I13" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="37"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9">
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9">
+      <c r="F14" s="8"/>
+      <c r="G14" s="8">
         <v>450000</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="I14" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="9">
+      <c r="B15" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="40">
         <v>103853</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9">
+      <c r="F15" s="8"/>
+      <c r="G15" s="8">
         <v>355000</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="9" t="s">
+      <c r="H15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
+      <c r="I15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="9">
+      <c r="B16" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="40">
         <v>377000</v>
       </c>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9">
+      <c r="D16" s="8"/>
+      <c r="E16" s="8">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9">
+      <c r="F16" s="8"/>
+      <c r="G16" s="8">
         <v>350000</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="9" t="s">
+      <c r="H16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="I16" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="9">
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="40">
         <v>92929</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9">
+      <c r="D17" s="8"/>
+      <c r="E17" s="8">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9">
+      <c r="F17" s="8"/>
+      <c r="G17" s="8">
         <v>350000</v>
       </c>
-      <c r="H17" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="9" t="s">
+      <c r="H17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="9">
+      <c r="I17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="40">
         <v>25246</v>
       </c>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9">
+      <c r="F18" s="8"/>
+      <c r="G18" s="8">
         <v>340000</v>
       </c>
-      <c r="H18" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I18" s="9" t="s">
+      <c r="H18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="I18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="9">
+      <c r="B19" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="40">
         <v>31123</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9">
+      <c r="D19" s="8"/>
+      <c r="E19" s="8">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9">
+      <c r="F19" s="8"/>
+      <c r="G19" s="8">
         <v>278000</v>
       </c>
-      <c r="H19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I19" s="9" t="s">
+      <c r="H19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="9" t="s">
+      <c r="I19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="40">
         <v>291634</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9">
+      <c r="D20" s="8"/>
+      <c r="E20" s="8">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9">
+      <c r="F20" s="8"/>
+      <c r="G20" s="8">
         <v>265000</v>
       </c>
-      <c r="H20" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="9" t="s">
+      <c r="H20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="22" t="s">
+      <c r="I20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="40">
         <v>21120</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="22">
+      <c r="D21" s="8"/>
+      <c r="E21" s="20">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="22">
+      <c r="F21" s="8"/>
+      <c r="G21" s="20">
         <v>240000</v>
       </c>
-      <c r="H21" s="23" t="s">
+      <c r="H21" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="24" t="s">
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="J21" s="9"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="22">
+      <c r="C22" s="40">
         <v>43975</v>
       </c>
-      <c r="D22" s="9">
+      <c r="D22" s="8">
         <v>50</v>
       </c>
-      <c r="E22" s="22">
+      <c r="E22" s="20">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="F22" s="9"/>
-      <c r="G22" s="22">
+      <c r="F22" s="8"/>
+      <c r="G22" s="20">
         <v>116000</v>
       </c>
-      <c r="H22" s="23" t="s">
+      <c r="H22" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="I22" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" s="9"/>
+      <c r="J22" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="16">
+    <mergeCell ref="C5:C10"/>
+    <mergeCell ref="B13:B14"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="J1:J3"/>
@@ -1451,11 +1529,12 @@
     <mergeCell ref="I1:I3"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="B1:B3"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="B5:B10"/>
-    <mergeCell ref="B1:B3"/>
     <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H4" r:id="rId1"/>

</xml_diff>

<commit_message>
přidána čerstvá data návštěvnosti libereckého bazénového komplexu
</commit_message>
<xml_diff>
--- a/src/kapacita/navstevnost_existujicich_bazenu.xlsx
+++ b/src/kapacita/navstevnost_existujicich_bazenu.xlsx
@@ -1,30 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\git\plavecky-stadion-prostejov\plavecky-stadion-prostejov\src\kapacita\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\git\janzilka\plavecky-stadion-prostejov\src\kapacita\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EA5653-FAB9-4C49-BCD9-4207331C1CB8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15900" yWindow="0" windowWidth="7650" windowHeight="7890"/>
+    <workbookView xWindow="1590" yWindow="-120" windowWidth="23730" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>Sušice</t>
   </si>
@@ -226,13 +233,19 @@
   <si>
     <t>aktuální data</t>
   </si>
+  <si>
+    <t>idnes.cz</t>
+  </si>
+  <si>
+    <t>roční návštěva výpočtem</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="###\ ###\ ##0"/>
+    <numFmt numFmtId="164" formatCode="###\ ###\ ##0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -442,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -503,6 +516,41 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -527,43 +575,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -600,7 +625,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -655,7 +686,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -677,6 +714,67 @@
         <a:xfrm>
           <a:off x="11534775" y="2209800"/>
           <a:ext cx="3581400" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4076700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>523875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C2BB42B-EBD7-443C-9B99-9A281B05B1A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="11944350" y="6019800"/>
+          <a:ext cx="3743325" cy="1133475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -960,14 +1058,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="F5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,56 +1080,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="39" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="24" t="s">
+      <c r="F1" s="44"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="37" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="25"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="25" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="30"/>
+      <c r="F2" s="43"/>
       <c r="G2" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="25"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="15" t="s">
         <v>18</v>
       </c>
@@ -1041,18 +1139,18 @@
       <c r="G3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" s="2" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="39">
+      <c r="C4" s="28">
         <v>11000</v>
       </c>
       <c r="D4" s="3">
@@ -1076,13 +1174,13 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="30">
         <v>90000</v>
       </c>
       <c r="D5" s="10">
@@ -1104,11 +1202,11 @@
       <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38" t="s">
+      <c r="A6" s="45"/>
+      <c r="B6" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="44"/>
+      <c r="C6" s="31"/>
       <c r="D6" s="10">
         <v>600</v>
       </c>
@@ -1124,11 +1222,11 @@
       <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="38" t="s">
+      <c r="A7" s="45"/>
+      <c r="B7" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="11">
         <v>680</v>
       </c>
@@ -1144,11 +1242,11 @@
       <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="38" t="s">
+      <c r="A8" s="45"/>
+      <c r="B8" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="44"/>
+      <c r="C8" s="31"/>
       <c r="D8" s="11">
         <v>370</v>
       </c>
@@ -1164,11 +1262,11 @@
       <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="38" t="s">
+      <c r="A9" s="45"/>
+      <c r="B9" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="44"/>
+      <c r="C9" s="31"/>
       <c r="D9" s="11">
         <v>60</v>
       </c>
@@ -1184,11 +1282,11 @@
       <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="37"/>
-      <c r="B10" s="38" t="s">
+      <c r="A10" s="45"/>
+      <c r="B10" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="45"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -1202,18 +1300,18 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C11" s="35">
         <v>1280000</v>
       </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8">
-        <f t="shared" ref="E11:E22" si="0">ROUNDDOWN(G11/365,-2)</f>
+        <f t="shared" ref="E11:E23" si="0">ROUNDDOWN(G11/365,-2)</f>
         <v>2600</v>
       </c>
       <c r="F11" s="8"/>
@@ -1229,11 +1327,11 @@
       <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36"/>
-      <c r="B12" s="34" t="s">
+      <c r="A12" s="34"/>
+      <c r="B12" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="42"/>
+      <c r="C12" s="36"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8">
         <f t="shared" si="0"/>
@@ -1252,13 +1350,13 @@
       <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="41">
+      <c r="C13" s="35">
         <v>170548</v>
       </c>
       <c r="D13" s="8"/>
@@ -1279,9 +1377,9 @@
       <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="42"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="34"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8">
         <f t="shared" si="0"/>
@@ -1299,14 +1397,14 @@
       </c>
       <c r="J14" s="8"/>
     </row>
-    <row r="15" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="38" t="s">
+    <row r="15" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="46">
         <v>103853</v>
       </c>
       <c r="D15" s="8"/>
@@ -1324,44 +1422,38 @@
       <c r="I15" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="J15" s="8"/>
-    </row>
-    <row r="16" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="40">
-        <v>377000</v>
-      </c>
+      <c r="J15" s="48"/>
+    </row>
+    <row r="16" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="34"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8">
-        <f t="shared" si="0"/>
-        <v>900</v>
+        <v>1100</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="8">
-        <v>350000</v>
+        <f>E16*365</f>
+        <v>401500</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J16" s="8"/>
+        <v>65</v>
+      </c>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="40">
-        <v>92929</v>
+      <c r="A17" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="29">
+        <v>377000</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="8">
@@ -1381,14 +1473,14 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="40">
-        <v>25246</v>
+      <c r="A18" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="29">
+        <v>92929</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8">
@@ -1397,7 +1489,7 @@
       </c>
       <c r="F18" s="8"/>
       <c r="G18" s="8">
-        <v>340000</v>
+        <v>350000</v>
       </c>
       <c r="H18" s="6" t="s">
         <v>45</v>
@@ -1408,23 +1500,23 @@
       <c r="J18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="40">
-        <v>31123</v>
+      <c r="A19" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="29">
+        <v>25246</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>900</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="8">
-        <v>278000</v>
+        <v>340000</v>
       </c>
       <c r="H19" s="6" t="s">
         <v>45</v>
@@ -1435,14 +1527,14 @@
       <c r="J19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="C20" s="40">
-        <v>291634</v>
+      <c r="A20" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="29">
+        <v>31123</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8">
@@ -1451,7 +1543,7 @@
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="8">
-        <v>265000</v>
+        <v>278000</v>
       </c>
       <c r="H20" s="6" t="s">
         <v>45</v>
@@ -1461,97 +1553,129 @@
       </c>
       <c r="J20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="38" t="s">
+    <row r="21" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="29">
+        <v>291634</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8">
+        <v>265000</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="30.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B22" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="40">
+      <c r="C22" s="29">
         <v>21120</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="20">
+      <c r="D22" s="8"/>
+      <c r="E22" s="20">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="20">
+      <c r="F22" s="8"/>
+      <c r="G22" s="20">
         <v>240000</v>
       </c>
-      <c r="H21" s="21" t="s">
+      <c r="H22" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="I22" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="J21" s="8"/>
-    </row>
-    <row r="22" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="s">
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="34" t="s">
+      <c r="B23" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="40">
+      <c r="C23" s="29">
         <v>43975</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D23" s="8">
         <v>50</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E23" s="20">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="20">
+      <c r="F23" s="8"/>
+      <c r="G23" s="20">
         <v>116000</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="H23" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="I23" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J22" s="8"/>
+      <c r="J23" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="20">
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="J1:J3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="I1:I3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="D2:D3"/>
     <mergeCell ref="C5:C10"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="H1:H3"/>
-    <mergeCell ref="J1:J3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="I1:I3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E1:G1"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A1:A3"/>
-    <mergeCell ref="D2:D3"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="A11:A12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H4" r:id="rId1"/>
-    <hyperlink ref="H5" r:id="rId2"/>
-    <hyperlink ref="H6" r:id="rId3"/>
-    <hyperlink ref="H7" r:id="rId4"/>
-    <hyperlink ref="H8" r:id="rId5"/>
-    <hyperlink ref="H9" r:id="rId6"/>
-    <hyperlink ref="H10" r:id="rId7"/>
-    <hyperlink ref="H11" r:id="rId8"/>
-    <hyperlink ref="H12:H20" r:id="rId9" display="aquainfo.cz"/>
-    <hyperlink ref="H21" r:id="rId10"/>
-    <hyperlink ref="H22" r:id="rId11"/>
-    <hyperlink ref="H14" r:id="rId12"/>
+    <hyperlink ref="H4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="H7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="H9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="H11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="H12:H21" r:id="rId9" display="aquainfo.cz" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="H22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H23" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H14" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="H16" r:id="rId13" xr:uid="{9F165400-8BD1-4A64-9F7D-01A53CF185D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
-  <drawing r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>